<commit_message>
Deploying to gh-pages from  @ f61b6b856fe916e5aba0a2d26945892c8efe815c 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/16.5.1.1a.xlsx
+++ b/en/downloads/data-excel/16.5.1.1a.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\ПоказателиЦУР для Платформы\Национальные показатели ЦУР\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\korozbaeva\Desktop\Показатели ЦУР для Платформы\Национальные показатели ЦУР\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -141,13 +141,13 @@
     <t>(points)</t>
   </si>
   <si>
-    <t>16.5.1.1a.Индекс "Личное представление об уровне коррупции в государственных органах исполнительной власти и органах местного самоуправления''</t>
+    <t>16.5.1.1a "Аткаруу бийлигинин мамлекеттик органдарындагы жана жергиликтүү өз алдынча башкаруу органдарындагы коррупциянын деңгээли жөнүндө жеке түшүнүк" индекси</t>
   </si>
   <si>
-    <t>16.5.1.1a."Аткаруу бийлигинин мамлекеттик органдарындагы жана жергиликтүү өз алдынча башкаруу органдарындагы коррупциянын деңгээли жөнүндө жеке түшүнүк" индекси</t>
+    <t>16.5.1.1a Индекс "Личное представление об уровне коррупции в государственных органах исполнительной власти и органах местного самоуправления''</t>
   </si>
   <si>
-    <t>16.5.1.1a.Index "Personal views about the level of corruption in executive government authorities and local government''</t>
+    <t>16.5.1.1a Index "Personal views about the level of corruption in executive government authorities and local government''</t>
   </si>
 </sst>
 </file>
@@ -344,7 +344,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -431,6 +431,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal 17" xfId="6"/>
@@ -8207,10 +8210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8220,19 +8223,19 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="59.25" customHeight="1">
+    <row r="1" spans="1:9" ht="59.25" customHeight="1">
       <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>38</v>
       </c>
       <c r="D1" s="17"/>
     </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1">
+    <row r="2" spans="1:9" ht="18" customHeight="1">
       <c r="A2" s="35" t="s">
         <v>33</v>
       </c>
@@ -8244,13 +8247,13 @@
       </c>
       <c r="D2" s="17"/>
     </row>
-    <row r="3" spans="1:8" ht="18" customHeight="1" thickBot="1">
+    <row r="3" spans="1:9" ht="18" customHeight="1" thickBot="1">
       <c r="A3" s="35"/>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1">
+    <row r="4" spans="1:9" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
@@ -8275,8 +8278,11 @@
       <c r="H4" s="20">
         <v>2019</v>
       </c>
+      <c r="I4" s="20">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" s="30" customFormat="1" ht="12.95" customHeight="1">
+    <row r="5" spans="1:9" s="30" customFormat="1" ht="12.95" customHeight="1">
       <c r="A5" s="29" t="s">
         <v>3</v>
       </c>
@@ -8301,8 +8307,11 @@
       <c r="H5" s="34">
         <v>14.1</v>
       </c>
+      <c r="I5" s="36">
+        <v>12.3</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" s="31" customFormat="1" ht="12.95" customHeight="1">
+    <row r="6" spans="1:9" s="31" customFormat="1" ht="12.95" customHeight="1">
       <c r="A6" s="14" t="s">
         <v>6</v>
       </c>
@@ -8327,8 +8336,11 @@
       <c r="H6" s="2">
         <v>37.4</v>
       </c>
+      <c r="I6" s="37">
+        <v>40.299999999999997</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" s="31" customFormat="1" ht="12.95" customHeight="1">
+    <row r="7" spans="1:9" s="31" customFormat="1" ht="12.95" customHeight="1">
       <c r="A7" s="14" t="s">
         <v>9</v>
       </c>
@@ -8353,8 +8365,11 @@
       <c r="H7" s="2">
         <v>40.799999999999997</v>
       </c>
+      <c r="I7" s="37">
+        <v>36.200000000000003</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" ht="12.95" customHeight="1">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="12.95" customHeight="1">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -8379,8 +8394,11 @@
       <c r="H8" s="2">
         <v>45.7</v>
       </c>
+      <c r="I8" s="37">
+        <v>44.3</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" ht="12.95" customHeight="1">
+    <row r="9" spans="1:9" s="2" customFormat="1" ht="12.95" customHeight="1">
       <c r="A9" s="12" t="s">
         <v>15</v>
       </c>
@@ -8405,8 +8423,11 @@
       <c r="H9" s="2">
         <v>24.6</v>
       </c>
+      <c r="I9" s="37">
+        <v>36</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="12.95" customHeight="1">
+    <row r="10" spans="1:9" s="2" customFormat="1" ht="12.95" customHeight="1">
       <c r="A10" s="12" t="s">
         <v>18</v>
       </c>
@@ -8431,8 +8452,11 @@
       <c r="H10" s="2">
         <v>12.6</v>
       </c>
+      <c r="I10" s="37">
+        <v>2.7</v>
+      </c>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" ht="12.95" customHeight="1">
+    <row r="11" spans="1:9" s="2" customFormat="1" ht="12.95" customHeight="1">
       <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
@@ -8457,8 +8481,11 @@
       <c r="H11" s="2">
         <v>29.5</v>
       </c>
+      <c r="I11" s="37">
+        <v>32.9</v>
+      </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" ht="12.95" customHeight="1">
+    <row r="12" spans="1:9" s="2" customFormat="1" ht="12.95" customHeight="1">
       <c r="A12" s="12" t="s">
         <v>24</v>
       </c>
@@ -8483,8 +8510,11 @@
       <c r="H12" s="2">
         <v>17.399999999999999</v>
       </c>
+      <c r="I12" s="37">
+        <v>11.3</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" ht="12.95" customHeight="1">
+    <row r="13" spans="1:9" s="2" customFormat="1" ht="12.95" customHeight="1">
       <c r="A13" s="14" t="s">
         <v>27</v>
       </c>
@@ -8509,8 +8539,11 @@
       <c r="H13" s="2">
         <v>-18</v>
       </c>
+      <c r="I13" s="37">
+        <v>-18.2</v>
+      </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" ht="12.95" customHeight="1" thickBot="1">
+    <row r="14" spans="1:9" s="2" customFormat="1" ht="12.95" customHeight="1" thickBot="1">
       <c r="A14" s="15" t="s">
         <v>29</v>
       </c>
@@ -8535,13 +8568,16 @@
       <c r="H14" s="33">
         <v>22.8</v>
       </c>
+      <c r="I14" s="38">
+        <v>33</v>
+      </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" s="2" customFormat="1" ht="12.95" customHeight="1">

</xml_diff>